<commit_message>
get 2022q1 of air quality
</commit_message>
<xml_diff>
--- a/administrative/main.xlsx
+++ b/administrative/main.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\pandemic_modelling\administrative\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\thesis\administrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF036AC-E6BA-4D56-81EC-36905EA58580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC4F899-A302-446E-B4F0-10C585E3F0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{4AC8BB16-67F5-4941-86E8-7E194268DB8A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{4AC8BB16-67F5-4941-86E8-7E194268DB8A}"/>
   </bookViews>
   <sheets>
     <sheet name="literature review" sheetId="1" r:id="rId1"/>
@@ -1962,7 +1962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA430712-2AF2-46BC-B2A9-A9F8B8AAD612}">
   <dimension ref="B1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -5553,7 +5553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE21AE24-7B23-4499-8D22-C9A70AD3E5F9}">
   <dimension ref="B1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add xgboost time series
</commit_message>
<xml_diff>
--- a/administrative/main.xlsx
+++ b/administrative/main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\thesis\administrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93E2156-DEC0-4550-B187-291F5295CF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37FB8B5-E76D-43B3-8A6F-90835019DEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{4AC8BB16-67F5-4941-86E8-7E194268DB8A}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="282">
   <si>
     <t>Pandemics &amp; Diffussion Models</t>
   </si>
@@ -907,6 +907,9 @@
   </si>
   <si>
     <t>do an svar after doing variable selection with lasso</t>
+  </si>
+  <si>
+    <t>kind of</t>
   </si>
 </sst>
 </file>
@@ -2177,7 +2180,7 @@
   <dimension ref="B1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2331,7 +2334,7 @@
         <v>255</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
@@ -2351,7 +2354,7 @@
         <v>256</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>253</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">

</xml_diff>